<commit_message>
saving persist in document class
</commit_message>
<xml_diff>
--- a/src/CaseStudy.xlsx
+++ b/src/CaseStudy.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -22,26 +22,29 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">Hi</t>
+    <t>Hi</t>
   </si>
   <si>
-    <t xml:space="preserve">I am Josh</t>
+    <t>I am Josh</t>
   </si>
   <si>
-    <t xml:space="preserve">Joshua was here</t>
+    <t>Joshua was Here!!</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello Outsourced! This text is created within the file.</t>
+    <t>Hello Outsourced! This text is created within the file.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -53,23 +56,6 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -80,7 +66,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalUp="1" diagonalDown="1">
       <left/>
       <right/>
       <top/>
@@ -88,58 +74,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" applyProtection="1"/>
+    <xf numFmtId="43" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyProtection="1"/>
+    <xf numFmtId="41" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyProtection="1"/>
+    <xf numFmtId="44" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyProtection="1"/>
+    <xf numFmtId="42" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyProtection="1"/>
+    <xf numFmtId="9" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -151,23 +110,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L2" s="0" t="s">
+    <row r="2" ht="15">
+      <c r="L2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M4" s="1" t="s">
+    <row r="4" ht="13.8">
+      <c r="M4" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" ht="15">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="2" t="s">
+    <row r="25" ht="15">
+      <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>